<commit_message>
Author : Sarthak 	Files Updated : database/DbSchema 	Files Added : database/sems_courses.sql, database/sems_instructors.sql, database/sems_session_details.sql 	Description : Updated Schema & Added Sql files to generated Db
</commit_message>
<xml_diff>
--- a/database/DbSchema.xlsx
+++ b/database/DbSchema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\SnB\prototype_application\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB05033E-7ED5-406C-87DA-FE2196505D6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47CAC1F-5FFF-409B-84AA-2DEE353FBE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9EE0F1A-AE7D-4BD3-8F06-185F8DDBBAD7}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>Instructors</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Table Name</t>
   </si>
@@ -51,9 +48,6 @@
     <t>Foreign Key</t>
   </si>
   <si>
-    <t>Courses</t>
-  </si>
-  <si>
     <t>course_id</t>
   </si>
   <si>
@@ -78,22 +72,25 @@
     <t>assesment_date</t>
   </si>
   <si>
-    <t>SessionDetails</t>
-  </si>
-  <si>
     <t>session_id</t>
   </si>
   <si>
     <t>session_name</t>
   </si>
   <si>
-    <t>session_date</t>
-  </si>
-  <si>
     <t>session_start_time</t>
   </si>
   <si>
     <t>session_end_time</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>instructors</t>
+  </si>
+  <si>
+    <t>session_details</t>
   </si>
 </sst>
 </file>
@@ -517,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE275330-B370-40D3-AA1D-C9B088C481C0}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,119 +528,115 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>2</v>
+      <c r="A22" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="512" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Author : Sarthak 	Files Added : database/sems_db.sql 	Files Updated : database/DbSchema.xlsx 	Files Deleted : database/sems_courses.sql, database/sems_instructors.sql, database/sems_session_details.sql 	Description : Updated Schema & Added Sql files & data to generated Db
</commit_message>
<xml_diff>
--- a/database/DbSchema.xlsx
+++ b/database/DbSchema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\SnB\prototype_application\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47CAC1F-5FFF-409B-84AA-2DEE353FBE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5536235-22EE-40A0-A432-0033E0236B98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9EE0F1A-AE7D-4BD3-8F06-185F8DDBBAD7}"/>
+    <workbookView xWindow="23550" yWindow="1215" windowWidth="10095" windowHeight="13125" xr2:uid="{C9EE0F1A-AE7D-4BD3-8F06-185F8DDBBAD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Table Name</t>
   </si>
@@ -91,13 +91,16 @@
   </si>
   <si>
     <t>session_details</t>
+  </si>
+  <si>
+    <t>course_img</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +115,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -188,10 +205,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -200,8 +218,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,34 +537,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE275330-B370-40D3-AA1D-C9B088C481C0}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -549,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -557,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -565,73 +594,78 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author : Sarthak 	Files Updated : database/DbSchema.xlsx 				,   database/sems_db.sql 	Description : Updated Db with Category Field
</commit_message>
<xml_diff>
--- a/database/DbSchema.xlsx
+++ b/database/DbSchema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\SnB\prototype_application\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5536235-22EE-40A0-A432-0033E0236B98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA39514D-221D-4A78-9B11-BF2A58CD9606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23550" yWindow="1215" windowWidth="10095" windowHeight="13125" xr2:uid="{C9EE0F1A-AE7D-4BD3-8F06-185F8DDBBAD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9EE0F1A-AE7D-4BD3-8F06-185F8DDBBAD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Table Name</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>course_img</t>
+  </si>
+  <si>
+    <t>course_category</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -204,12 +207,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -222,6 +234,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -537,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE275330-B370-40D3-AA1D-C9B088C481C0}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,42 +643,47 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>